<commit_message>
add col_info.py ColumnInfo.SetTblIndexList method; update projtables.py based on client version updates
</commit_message>
<xml_diff>
--- a/tests/test_data/col_info.xlsx
+++ b/tests/test_data/col_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_Col_Info\tests\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ModelingToolbox\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB77AA2-6BA3-46EA-B603-C2E2E25A2AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6394B6-7713-4F3B-BC35-7B5149F204D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="997" yWindow="930" windowWidth="17010" windowHeight="13657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="1110" windowWidth="28800" windowHeight="11587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cols" sheetId="5" r:id="rId1"/>

</xml_diff>

<commit_message>
Add validated parsetables.py ParseColMajorTbl class
</commit_message>
<xml_diff>
--- a/tests/test_data/col_info.xlsx
+++ b/tests/test_data/col_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ModelingToolbox\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6394B6-7713-4F3B-BC35-7B5149F204D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15214767-3311-48F8-862C-03A38785989F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="1110" windowWidth="28800" windowHeight="11587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1087" yWindow="1455" windowWidth="28801" windowHeight="11588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cols" sheetId="5" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>cols</t>
   </si>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>int64</t>
-  </si>
-  <si>
-    <t>datetime</t>
   </si>
 </sst>
 </file>
@@ -777,7 +774,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="H17" sqref="H17"/>
+      <selection pane="topRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1111,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="I14" s="12"/>
     </row>

</xml_diff>